<commit_message>
Added data validation for date
</commit_message>
<xml_diff>
--- a/240605_Doug_UDA_Unit7_Data_Cleaning_InClass_Exercise.xlsx
+++ b/240605_Doug_UDA_Unit7_Data_Cleaning_InClass_Exercise.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Student\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Student\UDA_tasks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8745D08C-DD8C-4721-B6B6-FEB9BC993015}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4E4602B-7BD9-44DF-A054-D788D94E42B7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{EE4959FF-4721-4E9C-B7AA-F4A6ED667D18}"/>
   </bookViews>
@@ -883,7 +883,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E85348C-5C8E-465E-A18C-C143DCA59690}">
   <dimension ref="A1:N15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1564,6 +1566,12 @@
       </c>
     </row>
   </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="date" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Must input Date bjbjbj" sqref="B1:B1048576" xr:uid="{D8FD6E44-2F21-41B1-A28D-CC8BFBD47427}">
+      <formula1>33219</formula1>
+      <formula2>44907</formula2>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
@@ -2085,7 +2093,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="19" spans="2:12" ht="45" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:12" ht="30" x14ac:dyDescent="0.25">
       <c r="B19" s="5">
         <v>202308241013</v>
       </c>
@@ -2119,7 +2127,7 @@
         <v>1260</v>
       </c>
     </row>
-    <row r="20" spans="2:12" ht="45" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:12" ht="30" x14ac:dyDescent="0.25">
       <c r="B20" s="5">
         <v>202308241013.60001</v>
       </c>
@@ -2725,7 +2733,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="19" spans="2:12" ht="45" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:12" ht="30" x14ac:dyDescent="0.25">
       <c r="B19" s="5">
         <v>202308241013</v>
       </c>
@@ -2759,7 +2767,7 @@
         <v>1260</v>
       </c>
     </row>
-    <row r="20" spans="2:12" ht="45" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:12" ht="30" x14ac:dyDescent="0.25">
       <c r="B20" s="5">
         <v>202308241013.60001</v>
       </c>

</xml_diff>